<commit_message>
update Tully army size data
</commit_message>
<xml_diff>
--- a/house_stats.xlsx
+++ b/house_stats.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savannahtjaden/Documents/github/GoT_shiny_app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C261B-0D2D-2F46-8B5A-C52E347BA9AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{B71D0E5D-098D-234A-88C9-B3823B4EABB5}"/>
+    <workbookView xWindow="384" yWindow="456" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="final_stats" sheetId="3" r:id="rId1"/>
@@ -20,9 +14,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$H$98</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="67">
   <si>
     <t>House</t>
   </si>
@@ -244,7 +238,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -335,7 +329,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Savannah Tjaden" refreshedDate="43523.613143171293" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="84" xr:uid="{4E54454E-48E3-1245-BBF3-5341C1E4A56A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Savannah Tjaden" refreshedDate="43523.613143171293" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="84">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G85" sheet="Sheet1"/>
   </cacheSource>
@@ -1201,7 +1195,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BDD7FF3-D178-9B45-829D-E913AF42AD6D}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1665,28 +1659,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650A8F98-1F7B-A545-B9D8-18B280FB380F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
@@ -1745,7 +1739,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1805,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1865,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1985,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2045,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2105,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2165,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2285,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2345,7 +2339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2465,7 +2459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2525,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2585,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2645,7 +2639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2705,7 +2699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2731,14 +2725,14 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>51</v>
+      <c r="I18" s="7">
+        <v>1000</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>51</v>
+      <c r="K18" s="7">
+        <v>10000</v>
       </c>
       <c r="L18" s="5">
         <v>0</v>
@@ -2771,20 +2765,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E0E5BA-5A1A-E543-9F58-C46CA59CC260}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2807,7 +2801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2830,7 +2824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2853,7 +2847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2873,7 +2867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2896,7 +2890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2919,7 +2913,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2942,7 +2936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2965,7 +2959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2988,7 +2982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -3011,7 +3005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3034,7 +3028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3057,7 +3051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3080,7 +3074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3103,7 +3097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -3126,7 +3120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -3146,7 +3140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7</v>
       </c>
@@ -3166,7 +3160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -3186,7 +3180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -3206,7 +3200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -3229,7 +3223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -3249,7 +3243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10</v>
       </c>
@@ -3272,7 +3266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10</v>
       </c>
@@ -3292,7 +3286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11</v>
       </c>
@@ -3315,7 +3309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>11</v>
       </c>
@@ -3338,7 +3332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -3361,7 +3355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12</v>
       </c>
@@ -3381,7 +3375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>13</v>
       </c>
@@ -3401,7 +3395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>13</v>
       </c>
@@ -3421,7 +3415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14</v>
       </c>
@@ -3444,7 +3438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>14</v>
       </c>
@@ -3467,7 +3461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -3490,7 +3484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>15</v>
       </c>
@@ -3513,7 +3507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -3536,7 +3530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -3559,7 +3553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>16</v>
       </c>
@@ -3585,7 +3579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16</v>
       </c>
@@ -3611,7 +3605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>17</v>
       </c>
@@ -3634,7 +3628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>17</v>
       </c>
@@ -3657,7 +3651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>18</v>
       </c>
@@ -3680,7 +3674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>18</v>
       </c>
@@ -3703,7 +3697,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>19</v>
       </c>
@@ -3726,7 +3720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>19</v>
       </c>
@@ -3746,7 +3740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>20</v>
       </c>
@@ -3769,7 +3763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20</v>
       </c>
@@ -3792,7 +3786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>21</v>
       </c>
@@ -3812,7 +3806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>21</v>
       </c>
@@ -3832,7 +3826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>22</v>
       </c>
@@ -3855,7 +3849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>22</v>
       </c>
@@ -3875,7 +3869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>24</v>
       </c>
@@ -3892,7 +3886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>24</v>
       </c>
@@ -3912,7 +3906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>25</v>
       </c>
@@ -3932,7 +3926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>25</v>
       </c>
@@ -3952,7 +3946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>26</v>
       </c>
@@ -3975,7 +3969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>26</v>
       </c>
@@ -3998,7 +3992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>26</v>
       </c>
@@ -4021,7 +4015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>27</v>
       </c>
@@ -4041,7 +4035,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>27</v>
       </c>
@@ -4061,7 +4055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>28</v>
       </c>
@@ -4084,7 +4078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>28</v>
       </c>
@@ -4107,7 +4101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>29</v>
       </c>
@@ -4127,7 +4121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>29</v>
       </c>
@@ -4147,7 +4141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>31</v>
       </c>
@@ -4170,7 +4164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>31</v>
       </c>
@@ -4193,7 +4187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>31</v>
       </c>
@@ -4216,7 +4210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>31</v>
       </c>
@@ -4239,7 +4233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>31</v>
       </c>
@@ -4262,7 +4256,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>32</v>
       </c>
@@ -4282,7 +4276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>32</v>
       </c>
@@ -4302,7 +4296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>33</v>
       </c>
@@ -4322,7 +4316,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>33</v>
       </c>
@@ -4342,7 +4336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>34</v>
       </c>
@@ -4365,7 +4359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>34</v>
       </c>
@@ -4388,7 +4382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>36</v>
       </c>
@@ -4411,7 +4405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>36</v>
       </c>
@@ -4434,7 +4428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>36</v>
       </c>
@@ -4454,7 +4448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>37</v>
       </c>
@@ -4477,7 +4471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>37</v>
       </c>
@@ -4500,7 +4494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>37</v>
       </c>
@@ -4520,7 +4514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>38</v>
       </c>
@@ -4543,7 +4537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>38</v>
       </c>
@@ -4566,7 +4560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>38</v>
       </c>
@@ -4589,7 +4583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>38</v>
       </c>
@@ -4612,7 +4606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>38</v>
       </c>
@@ -4635,7 +4629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>38</v>
       </c>
@@ -4658,7 +4652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="1"/>
     </row>
   </sheetData>
@@ -4667,36 +4661,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5465F0B-F96E-7848-9A17-F5650F093AF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB98"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:AC19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.796875" customWidth="1"/>
+    <col min="11" max="11" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="15" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4755,7 +4749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
         <v>6</v>
       </c>
@@ -4815,7 +4809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -4881,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4947,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -5011,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -5077,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -5143,7 +5137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -5207,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -5271,7 +5265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5337,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -5403,7 +5397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -5469,7 +5463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -5535,7 +5529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -5601,7 +5595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -5667,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -5731,7 +5725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -5797,7 +5791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -5863,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -5871,13 +5865,13 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -5885,18 +5879,18 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J23" s="1"/>
     </row>
-    <row r="41" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="10:13" x14ac:dyDescent="0.3">
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
-    <row r="43" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J43" s="1"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="1"/>
     </row>
   </sheetData>

</xml_diff>